<commit_message>
adding kulldorff notes and state boundaries
</commit_message>
<xml_diff>
--- a/results/tables/most_significant_clusters.xlsx
+++ b/results/tables/most_significant_clusters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>LOC_ID</t>
   </si>
@@ -38,12 +38,6 @@
     <t>RADIUS</t>
   </si>
   <si>
-    <t>START_DATE</t>
-  </si>
-  <si>
-    <t>END_DATE</t>
-  </si>
-  <si>
     <t>NUMBER_LOC</t>
   </si>
   <si>
@@ -81,6 +75,9 @@
   </si>
   <si>
     <t>SatScan No Overlap Cluster</t>
+  </si>
+  <si>
+    <t>SpatialEpi Cluster</t>
   </si>
 </sst>
 </file>
@@ -104,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,6 +124,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -136,10 +144,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -422,81 +430,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -504,153 +508,166 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
         <v>36059</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>40.741750000000003</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>-73.589089999999999</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>68.0547749264</v>
       </c>
-      <c r="G2" s="2">
-        <v>43852</v>
-      </c>
-      <c r="H2" s="2">
-        <v>44044</v>
+      <c r="H2" s="1">
+        <v>15</v>
       </c>
       <c r="I2" s="1">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1">
         <v>97983.066700117299</v>
       </c>
-      <c r="K2" s="3">
+      <c r="J2" s="2">
         <v>1.0000000000000001E-17</v>
       </c>
+      <c r="K2" s="1">
+        <v>469091</v>
+      </c>
       <c r="L2" s="1">
-        <v>469091</v>
+        <v>233805.598228021</v>
       </c>
       <c r="M2" s="1">
-        <v>233805.598228021</v>
+        <v>2.0063292049000001</v>
       </c>
       <c r="N2" s="1">
-        <v>2.0063292049000001</v>
+        <v>2.1239253500999999</v>
       </c>
       <c r="O2" s="1">
-        <v>2.1239253500999999</v>
-      </c>
-      <c r="P2" s="1">
         <v>16949211</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>15</v>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
         <v>36005</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>40.85266</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>-73.866829999999993</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>36.289991326600003</v>
       </c>
-      <c r="G3" s="2">
-        <v>43852</v>
-      </c>
-      <c r="H3" s="2">
-        <v>44044</v>
+      <c r="H3" s="1">
+        <v>10</v>
       </c>
       <c r="I3" s="1">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
         <v>73915.560865669206</v>
       </c>
-      <c r="K3" s="3">
+      <c r="J3" s="2">
         <v>1.0000000000000001E-17</v>
       </c>
+      <c r="K3" s="1">
+        <v>359554</v>
+      </c>
       <c r="L3" s="1">
-        <v>359554</v>
+        <v>179145.346702343</v>
       </c>
       <c r="M3" s="1">
-        <v>179145.346702343</v>
+        <v>2.0070518527000001</v>
       </c>
       <c r="N3" s="1">
-        <v>2.0070518527000001</v>
+        <v>2.0948570146000001</v>
       </c>
       <c r="O3" s="1">
-        <v>2.0948570146000001</v>
-      </c>
-      <c r="P3" s="1">
         <v>12986739</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>16</v>
+      <c r="P3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
         <v>12045</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>29.955909999999999</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>-85.226669999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>734.35406356980002</v>
       </c>
-      <c r="G4" s="2">
-        <v>43852</v>
-      </c>
-      <c r="H4" s="2">
-        <v>44044</v>
+      <c r="H4" s="1">
+        <v>569</v>
       </c>
       <c r="I4" s="1">
-        <v>569</v>
-      </c>
-      <c r="J4" s="1">
         <v>67061.638033456606</v>
       </c>
-      <c r="K4" s="3">
+      <c r="J4" s="2">
         <v>1.0000000000000001E-17</v>
       </c>
+      <c r="K4" s="1">
+        <v>1093125</v>
+      </c>
       <c r="L4" s="1">
-        <v>1093125</v>
+        <v>784932.84176122095</v>
       </c>
       <c r="M4" s="1">
-        <v>784932.84176122095</v>
+        <v>1.3926350661</v>
       </c>
       <c r="N4" s="1">
-        <v>1.3926350661</v>
+        <v>1.5192345473</v>
       </c>
       <c r="O4" s="1">
-        <v>1.5192345473</v>
-      </c>
-      <c r="P4" s="1">
         <v>56901941</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>15</v>
+      <c r="P4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>599</v>
+      </c>
+      <c r="I5" s="3">
+        <v>69847.64</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1115105</v>
+      </c>
+      <c r="L5" s="3">
+        <v>798430.5</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1.3966209999999999</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1.5279290000000001</v>
+      </c>
+      <c r="O5" s="3">
+        <v>57880420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>